<commit_message>
Día 3: Agregue la version final de los casos de Prueba con su Ejecucion
</commit_message>
<xml_diff>
--- a/casos_de_prueba/matriz_pruebas.xlsx
+++ b/casos_de_prueba/matriz_pruebas.xlsx
@@ -994,7 +994,38 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE24040"/>
+          <bgColor rgb="FFE24040"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA4F05B"/>
+          <bgColor rgb="FFA4F05B"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF5E34A"/>
+          <bgColor rgb="FFF5E34A"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -2266,6 +2297,21 @@
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="E2:I2"/>
   </mergeCells>
+  <conditionalFormatting sqref="I1:I996">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"❌FAIL"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I996">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"✅OK"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I996">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"⚠BLOQUEADO"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I4:I20 I22:I36">
       <formula1>"❌FAIL,✅OK,⚠BLOQUEADO"</formula1>

</xml_diff>